<commit_message>
For README H/W submission
</commit_message>
<xml_diff>
--- a/Joseph_Mungoma_Week2Homework rework.xlsx
+++ b/Joseph_Mungoma_Week2Homework rework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e1458623\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\code\SavvyCoders\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41A0B2A-2A4D-4EBA-9DC0-468123982DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FC1DA3-32EA-4F08-BC19-BE301B148867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payments" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -924,15 +924,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -975,7 +976,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -996,15 +996,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -1025,15 +1016,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1045,30 +1045,45 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="40% - Accent4" xfId="3" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
     <cellStyle name="60% - Accent3" xfId="2" builtinId="40"/>
     <cellStyle name="60% - Accent4" xfId="4" builtinId="44"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="31">
     <dxf>
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <alignment vertical="top"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0"/>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
@@ -1077,46 +1092,16 @@
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0"/>
+      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
     </dxf>
     <dxf>
-      <alignment wrapText="0"/>
+      <alignment wrapText="1"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="0"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
@@ -1365,6 +1350,12 @@
       </border>
     </dxf>
     <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="top"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
@@ -1397,7 +1388,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Joseph_Mungoma_Week2Homework.xlsx]Payments!PivotTable4</c:name>
+    <c:name>[Joseph_Mungoma_Week2Homework rework.xlsx]Payments!PivotTable4</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -2593,19 +2584,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>14666.666666666666</c:v>
+                  <c:v>806.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3900</c:v>
+                  <c:v>187.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9100</c:v>
+                  <c:v>412.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>575</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6760</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3025,19 +3016,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>14666.666666666666</c:v>
+                  <c:v>806.66666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3900</c:v>
+                  <c:v>187.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9100</c:v>
+                  <c:v>412.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8000</c:v>
+                  <c:v>575</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6760</c:v>
+                  <c:v>325</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7561,7 +7552,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85616B58-18BA-40A2-A9D7-9A4CCC17CD32}" name="PivotTable4" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" colHeaderCaption="Bank Code">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{85616B58-18BA-40A2-A9D7-9A4CCC17CD32}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4" colHeaderCaption="Bank Code">
   <location ref="A3:E21" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField numFmtId="14" showAll="0"/>
@@ -7810,11 +7801,11 @@
   <dataFields count="1">
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="11" baseItem="0" numFmtId="164"/>
   </dataFields>
-  <formats count="6">
-    <format dxfId="36">
+  <formats count="16">
+    <format dxfId="30">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="29">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -7823,13 +7814,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="5">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="2">
+    <format dxfId="28">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -7841,7 +7826,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="27">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="6" count="1" selected="0">
@@ -7852,6 +7837,50 @@
           </reference>
         </references>
       </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="11">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="10">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="9">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="8">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="6">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="4">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="3">
+      <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="2">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
   <chartFormats count="6">
@@ -7952,18 +7981,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BF92EAE-EADA-4CD1-BD2A-2B0987FC034F}" name="Table1" displayName="Table1" ref="A2:I210" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9BF92EAE-EADA-4CD1-BD2A-2B0987FC034F}" name="Table1" displayName="Table1" ref="A2:I210" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23">
   <autoFilter ref="A2:I210" xr:uid="{9BF92EAE-EADA-4CD1-BD2A-2B0987FC034F}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{F821F615-1645-4413-8D10-7A128680982A}" name="Document Date" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{0C382D41-B173-4611-873D-F99185544EAF}" name="Supplier" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{E1BC6C76-E9E0-4C0F-9F8D-1E9EFD0EEE57}" name="Reference" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{C529623F-6144-44F0-84EA-6794773EEB21}" name="Description" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{58A325A9-748E-4621-8AE9-9DB64B4396AF}" name="Tax Inclusive Amount" dataDxfId="26" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{E25D0CA6-795D-4F60-A3CF-83D21DB2F70B}" name="Column1" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{399F12C1-C226-4CEB-961A-A16AACA0D3B1}" name="Bank Code" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{FA6BED4C-706B-4429-BC1F-532E833DC986}" name="Account Code" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{C7CB177B-3FFC-4CAB-809B-94536A136133}" name="Payment Date" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{F821F615-1645-4413-8D10-7A128680982A}" name="Document Date" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{0C382D41-B173-4611-873D-F99185544EAF}" name="Supplier" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{E1BC6C76-E9E0-4C0F-9F8D-1E9EFD0EEE57}" name="Reference" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{C529623F-6144-44F0-84EA-6794773EEB21}" name="Description" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{58A325A9-748E-4621-8AE9-9DB64B4396AF}" name="Tax Inclusive Amount" dataDxfId="18" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{E25D0CA6-795D-4F60-A3CF-83D21DB2F70B}" name="Column1" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{399F12C1-C226-4CEB-961A-A16AACA0D3B1}" name="Bank Code" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{FA6BED4C-706B-4429-BC1F-532E833DC986}" name="Account Code" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{C7CB177B-3FFC-4CAB-809B-94536A136133}" name="Payment Date" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8266,10 +8295,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1164E1C-0D45-4ED1-A991-F855665B857C}">
-  <dimension ref="A3:E21"/>
+  <dimension ref="A3:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8277,273 +8306,278 @@
     <col min="1" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:6" ht="30">
+      <c r="A3" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="49" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="18" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="49" t="s">
         <v>166</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="50" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="19">
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="18">
         <v>40910</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>1000</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="19">
+    <row r="6" spans="1:6">
+      <c r="A6" s="18">
         <v>40913</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>340</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21">
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20">
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="19">
+    <row r="7" spans="1:6">
+      <c r="A7" s="18">
         <v>40923</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>80</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="23">
         <v>35</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="19">
+    <row r="8" spans="1:6">
+      <c r="A8" s="18">
         <v>40924</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>1392</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="23">
+      <c r="C8" s="20"/>
+      <c r="D8" s="22">
         <v>105</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>1497</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="19">
+    <row r="9" spans="1:6">
+      <c r="A9" s="18">
         <v>40928</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>20000</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <v>-20000</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21">
+      <c r="D9" s="20"/>
+      <c r="E9" s="20">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="19">
+    <row r="10" spans="1:6">
+      <c r="A10" s="18">
         <v>40929</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20">
         <v>61</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="19">
+    <row r="11" spans="1:6">
+      <c r="A11" s="18">
         <v>40934</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <v>6720</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="20">
         <v>20000</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20">
         <v>26720</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="19">
+    <row r="12" spans="1:6">
+      <c r="A12" s="18">
         <v>40939</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>738.25</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21">
+      <c r="C12" s="20"/>
+      <c r="D12" s="20">
         <v>-170</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>568.25</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="19">
+    <row r="13" spans="1:6">
+      <c r="A13" s="18">
         <v>40941</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="20">
         <v>1000</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20">
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="19">
+    <row r="14" spans="1:6">
+      <c r="A14" s="18">
         <v>40944</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="20">
         <v>340</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20">
         <v>340</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="19">
+    <row r="15" spans="1:6">
+      <c r="A15" s="18">
         <v>40954</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="20">
         <v>80</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <v>35</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21">
+      <c r="D15" s="20"/>
+      <c r="E15" s="20">
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="19">
+    <row r="16" spans="1:6">
+      <c r="A16" s="18">
         <v>40959</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>20000</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <v>-20000</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21">
+      <c r="D16" s="20"/>
+      <c r="E16" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="19">
+      <c r="A17" s="18">
         <v>40964</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>2200</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20">
         <v>75</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <v>2275</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <v>40965</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="20">
         <v>6720</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="20">
         <v>20000</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20">
         <v>26720</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>40966</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="20">
         <v>514</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20">
         <v>514</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="19">
+      <c r="A20" s="18">
         <v>40968</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="20">
         <v>3770</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21">
+      <c r="C20" s="20"/>
+      <c r="D20" s="20">
         <v>-70</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="20">
         <v>3700</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="20">
         <v>64894.25</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="20">
         <v>70</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="20">
         <v>1</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="20">
         <v>64965.25</v>
       </c>
     </row>
@@ -14660,13 +14694,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1">
       <c r="A2" s="42"/>
@@ -14676,252 +14710,252 @@
       <c r="E2" s="42"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="31" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="33">
         <v>12</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="33">
         <v>85</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="26" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="35">
         <v>11</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="35">
         <v>72</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="35">
         <v>13</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="35">
         <v>60</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="35">
         <v>12</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="35">
         <v>95</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="35">
         <v>14</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="35">
         <v>88</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="35">
         <v>12</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="35">
         <v>99</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="35">
         <v>11</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="35">
         <v>75</v>
       </c>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="35">
         <v>13</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="35">
         <v>100</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="35">
         <v>13</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="35">
         <v>75</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="35">
         <v>15</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="35">
         <v>85</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="27" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="37">
         <v>11</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="37">
         <v>85</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="28" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="24">
         <f>MIN(C4:C14)</f>
         <v>11</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="24">
         <f>MIN(D4:D14)</f>
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="24">
         <f>MAX(C4:C14)</f>
         <v>15</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="24">
         <f>MAX(D4:D14)</f>
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="24">
         <f>AVERAGE(C4:C14)</f>
         <v>12.454545454545455</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="24">
         <f>AVERAGE(D4:D14)</f>
         <v>83.545454545454547</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="24">
         <f>MODE(C4:C14)</f>
         <v>12</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="24">
         <f>MODE(D4:D14)</f>
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="26" t="s">
+      <c r="A20" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="24">
         <f>MEDIAN(C4:C14)</f>
         <v>12</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="24">
         <f>MEDIAN(D4:D14)</f>
         <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="25" t="s">
         <v>150</v>
       </c>
       <c r="B21">
         <f>COUNT(B4:B14,C4:C14)</f>
         <v>11</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -14938,7 +14972,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14953,7 +14987,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="43" t="s">
         <v>152</v>
       </c>
       <c r="B1" s="44"/>
@@ -14964,34 +14998,34 @@
       <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="47"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
     </row>
     <row r="3" spans="1:7" ht="15.75">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="G3" s="43" t="s">
+      <c r="G3" s="38" t="s">
         <v>159</v>
       </c>
     </row>
@@ -15002,23 +15036,23 @@
       <c r="B4">
         <v>2000</v>
       </c>
-      <c r="C4" s="21">
-        <v>21</v>
+      <c r="C4" s="52">
+        <v>0.21</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4">
         <f>PRODUCT(B4*C4)</f>
-        <v>42000</v>
+        <v>420</v>
       </c>
       <c r="F4">
         <f>SUM(B4+E4)</f>
-        <v>44000</v>
+        <v>2420</v>
       </c>
       <c r="G4">
         <f>F4/D4</f>
-        <v>14666.666666666666</v>
+        <v>806.66666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -15028,23 +15062,23 @@
       <c r="B5">
         <v>450</v>
       </c>
-      <c r="C5" s="21">
-        <v>25</v>
+      <c r="C5" s="51">
+        <v>0.25</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E8" si="0">PRODUCT(B5*C5)</f>
-        <v>11250</v>
+        <v>112.5</v>
       </c>
       <c r="F5">
         <f t="shared" ref="F5:F8" si="1">SUM(B5+E5)</f>
-        <v>11700</v>
+        <v>562.5</v>
       </c>
       <c r="G5">
         <f>F5/D5</f>
-        <v>3900</v>
+        <v>187.5</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -15054,23 +15088,23 @@
       <c r="B6">
         <v>975</v>
       </c>
-      <c r="C6" s="21">
-        <v>27</v>
+      <c r="C6" s="51">
+        <v>0.27</v>
       </c>
       <c r="D6">
         <v>3</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>26325</v>
+        <v>263.25</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>27300</v>
+        <v>1238.25</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:G8" si="2">F6/D6</f>
-        <v>9100</v>
+        <v>412.75</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -15080,23 +15114,23 @@
       <c r="B7">
         <v>1500</v>
       </c>
-      <c r="C7" s="21">
-        <v>15</v>
+      <c r="C7" s="51">
+        <v>0.15</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>22500</v>
+        <v>225</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>24000</v>
+        <v>1725</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>8000</v>
+        <v>575</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -15106,23 +15140,23 @@
       <c r="B8">
         <v>780</v>
       </c>
-      <c r="C8" s="21">
-        <v>25</v>
+      <c r="C8" s="51">
+        <v>0.25</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>19500</v>
+        <v>195</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>20280</v>
+        <v>975</v>
       </c>
       <c r="G8">
         <f t="shared" si="2"/>
-        <v>6760</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>